<commit_message>
Added git rebase to cheatsheet
</commit_message>
<xml_diff>
--- a/DevOps_Cheatsheet.xlsx
+++ b/DevOps_Cheatsheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="1498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="1533">
   <si>
     <t>CREATING OBJECTS</t>
   </si>
@@ -5513,6 +5513,347 @@
   </si>
   <si>
     <t>GIT CONFIG</t>
+  </si>
+  <si>
+    <t>GIT REBASE</t>
+  </si>
+  <si>
+    <t>git rebase &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>Applies commits from the current branch on top of the specified branch, integrating the changes from both branches.</t>
+  </si>
+  <si>
+    <t>git rebase --continue</t>
+  </si>
+  <si>
+    <t>Continues the rebase operation after resolving conflicts in the current commit.</t>
+  </si>
+  <si>
+    <t>git rebase --skip</t>
+  </si>
+  <si>
+    <t>Skips the current commit during a rebase operation.</t>
+  </si>
+  <si>
+    <t>git rebase --abort</t>
+  </si>
+  <si>
+    <t>Aborts the ongoing rebase operation, restoring the branch to its state before the rebase started.</t>
+  </si>
+  <si>
+    <t>git rebase -i &lt;commit&gt;</t>
+  </si>
+  <si>
+    <t>Initiates an interactive rebase, allowing you to edit, reorder, squash, or drop commits before applying them.</t>
+  </si>
+  <si>
+    <t>git rebase --onto &lt;new-base&gt; &lt;old-base&gt;</t>
+  </si>
+  <si>
+    <t>git rebase --skip-if-unchanged &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>Skips rebasing if the branch has no new changes, allowing you to avoid unnecessary rebases.</t>
+  </si>
+  <si>
+    <t>git rebase --root</t>
+  </si>
+  <si>
+    <t>Rebases all commits from the root commit of the repository up to the current branch's tip.</t>
+  </si>
+  <si>
+    <t>git rebase --exec &lt;command&gt;</t>
+  </si>
+  <si>
+    <t>Runs the specified command after applying each commit during a rebase operation.</t>
+  </si>
+  <si>
+    <t>git rebase --ignore-date</t>
+  </si>
+  <si>
+    <t>Ignores commit dates and applies commits in the order they appear during a rebase operation.</t>
+  </si>
+  <si>
+    <t>git rebase --autostash</t>
+  </si>
+  <si>
+    <t>Automatically stashes and unstashes local changes before and after a rebase operation.</t>
+  </si>
+  <si>
+    <t>git rebase --strategy &lt;strategy&gt;</t>
+  </si>
+  <si>
+    <t>git rebase --strategy-option &lt;option&gt;</t>
+  </si>
+  <si>
+    <t>Specifies additional options for the selected merge strategy during a rebase operation.</t>
+  </si>
+  <si>
+    <t>git rebase --preserve-merges</t>
+  </si>
+  <si>
+    <t>Preserves merge commits during a rebase operation, instead of flattening them into individual commits.</t>
+  </si>
+  <si>
+    <t>git rebase --onto &lt;new-base&gt; &lt;old-base&gt; &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>git rebase --fork-point &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>git rebase --skip-empty</t>
+  </si>
+  <si>
+    <t>Skips applying empty commits during a rebase operation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Moves a range of commits from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;old-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;new-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, replaying the commits on top of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;new-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Specifies the merge strategy to be used during a rebase operation. Common strategies include </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>recursive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (default), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>resolve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>theirs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and more.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Moves a range of commits from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;old-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;new-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the specified </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;branch&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, replaying the commits on top of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;new-base&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Replays commits starting from the common ancestor of the current branch and the specified </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;branch&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ignoring commits that are already in the upstream branch.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6187,10 +6528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B419"/>
+  <dimension ref="A1:B439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
+      <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7971,1224 +8312,1373 @@
         <v>1193</v>
       </c>
     </row>
+    <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="3" t="s">
+        <v>1498</v>
+      </c>
+    </row>
     <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A248" s="3" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="21" t="s">
+      <c r="A248" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B249" s="22" t="s">
+      <c r="B248" s="22" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B249" t="s">
+        <v>1500</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>1029</v>
+        <v>1501</v>
       </c>
       <c r="B250" t="s">
-        <v>1030</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>1031</v>
+        <v>1503</v>
       </c>
       <c r="B251" t="s">
-        <v>1032</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>1033</v>
+        <v>1505</v>
       </c>
       <c r="B252" t="s">
-        <v>1034</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1035</v>
+        <v>1507</v>
       </c>
       <c r="B253" t="s">
-        <v>1036</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>1037</v>
+        <v>1509</v>
       </c>
       <c r="B254" t="s">
-        <v>1038</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>1039</v>
+        <v>1510</v>
       </c>
       <c r="B255" t="s">
-        <v>1040</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>1041</v>
+        <v>1512</v>
       </c>
       <c r="B256" t="s">
-        <v>1042</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>1043</v>
+        <v>1514</v>
       </c>
       <c r="B257" t="s">
-        <v>1044</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>1045</v>
+        <v>1516</v>
       </c>
       <c r="B258" t="s">
-        <v>1046</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>1047</v>
+        <v>1518</v>
       </c>
       <c r="B259" t="s">
-        <v>1048</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>1049</v>
+        <v>1520</v>
       </c>
       <c r="B260" t="s">
-        <v>1050</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>1051</v>
+        <v>1521</v>
       </c>
       <c r="B261" t="s">
-        <v>1052</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>1053</v>
+        <v>1523</v>
       </c>
       <c r="B262" t="s">
-        <v>1054</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>1055</v>
+        <v>1525</v>
       </c>
       <c r="B263" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A266" s="3" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A267" s="21" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B264" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B265" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A268" s="3" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A269" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B267" s="22" t="s">
+      <c r="B269" s="22" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B268" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B269" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>1203</v>
+        <v>1029</v>
       </c>
       <c r="B270" t="s">
-        <v>1204</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>1205</v>
+        <v>1031</v>
       </c>
       <c r="B271" t="s">
-        <v>1206</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>1207</v>
+        <v>1033</v>
       </c>
       <c r="B272" t="s">
-        <v>1208</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>1209</v>
+        <v>1035</v>
       </c>
       <c r="B273" t="s">
-        <v>1210</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>1211</v>
+        <v>1037</v>
       </c>
       <c r="B274" t="s">
-        <v>1212</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>1213</v>
+        <v>1039</v>
       </c>
       <c r="B275" t="s">
-        <v>1214</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>1215</v>
+        <v>1041</v>
       </c>
       <c r="B276" t="s">
-        <v>1216</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>1217</v>
+        <v>1043</v>
       </c>
       <c r="B277" t="s">
-        <v>1218</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>1219</v>
+        <v>1045</v>
       </c>
       <c r="B278" t="s">
-        <v>1220</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>1221</v>
+        <v>1047</v>
       </c>
       <c r="B279" t="s">
-        <v>1222</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>1223</v>
+        <v>1049</v>
       </c>
       <c r="B280" t="s">
-        <v>1224</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>1225</v>
+        <v>1051</v>
       </c>
       <c r="B281" t="s">
-        <v>1226</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>1227</v>
+        <v>1053</v>
       </c>
       <c r="B282" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A285" s="3" t="s">
-        <v>1229</v>
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A286" s="21" t="s">
+      <c r="A286" s="3" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A287" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B286" s="22" t="s">
+      <c r="B287" s="22" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B287" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>1231</v>
+        <v>1128</v>
       </c>
       <c r="B288" t="s">
-        <v>1232</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>1233</v>
+        <v>1201</v>
       </c>
       <c r="B289" t="s">
-        <v>1232</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>1234</v>
+        <v>1203</v>
       </c>
       <c r="B290" t="s">
-        <v>1235</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>1236</v>
+        <v>1205</v>
       </c>
       <c r="B291" t="s">
-        <v>1237</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>1238</v>
+        <v>1207</v>
       </c>
       <c r="B292" t="s">
-        <v>1239</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>1240</v>
+        <v>1209</v>
       </c>
       <c r="B293" t="s">
-        <v>1241</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>1242</v>
+        <v>1211</v>
       </c>
       <c r="B294" t="s">
-        <v>1243</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>1244</v>
+        <v>1213</v>
       </c>
       <c r="B295" t="s">
-        <v>1245</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>1246</v>
+        <v>1215</v>
       </c>
       <c r="B296" t="s">
-        <v>1247</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>1248</v>
+        <v>1217</v>
       </c>
       <c r="B297" t="s">
-        <v>1235</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>1249</v>
+        <v>1219</v>
       </c>
       <c r="B298" t="s">
-        <v>1250</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>1251</v>
+        <v>1221</v>
       </c>
       <c r="B299" t="s">
-        <v>1252</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>1253</v>
+        <v>1223</v>
       </c>
       <c r="B300" t="s">
-        <v>1254</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>1255</v>
+        <v>1225</v>
       </c>
       <c r="B301" t="s">
-        <v>1256</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>1257</v>
+        <v>1227</v>
       </c>
       <c r="B302" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" t="s">
-        <v>1259</v>
-      </c>
-      <c r="B303" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B304" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A307" s="3" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A308" s="21" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A305" s="3" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A306" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B308" s="22" t="s">
+      <c r="B306" s="22" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1232</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>1136</v>
+        <v>1233</v>
       </c>
       <c r="B309" t="s">
-        <v>1264</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>1265</v>
+        <v>1234</v>
       </c>
       <c r="B310" t="s">
-        <v>1266</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>1267</v>
+        <v>1236</v>
       </c>
       <c r="B311" t="s">
-        <v>1268</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>1269</v>
+        <v>1238</v>
       </c>
       <c r="B312" t="s">
-        <v>1270</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>1271</v>
+        <v>1240</v>
       </c>
       <c r="B313" t="s">
-        <v>1272</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>1273</v>
+        <v>1242</v>
       </c>
       <c r="B314" t="s">
-        <v>1274</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>1275</v>
+        <v>1244</v>
       </c>
       <c r="B315" t="s">
-        <v>1276</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>1277</v>
+        <v>1246</v>
       </c>
       <c r="B316" t="s">
-        <v>1278</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>1279</v>
+        <v>1248</v>
       </c>
       <c r="B317" t="s">
-        <v>1280</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>1281</v>
+        <v>1249</v>
       </c>
       <c r="B318" t="s">
-        <v>1282</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>1283</v>
+        <v>1251</v>
       </c>
       <c r="B319" t="s">
-        <v>1284</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>1285</v>
+        <v>1253</v>
       </c>
       <c r="B320" t="s">
-        <v>1286</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>1287</v>
+        <v>1255</v>
       </c>
       <c r="B321" t="s">
-        <v>1288</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>1289</v>
+        <v>1257</v>
       </c>
       <c r="B322" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A325" s="3" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A326" s="21" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A327" s="3" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A328" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B326" s="22" t="s">
+      <c r="B328" s="22" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A327" t="s">
-        <v>1292</v>
-      </c>
-      <c r="B327" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A328" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B328" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>1153</v>
+        <v>1136</v>
       </c>
       <c r="B329" t="s">
-        <v>1295</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>1296</v>
+        <v>1265</v>
       </c>
       <c r="B330" t="s">
-        <v>1297</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>1155</v>
+        <v>1267</v>
       </c>
       <c r="B331" t="s">
-        <v>1298</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>1299</v>
+        <v>1269</v>
       </c>
       <c r="B332" t="s">
-        <v>1300</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>1134</v>
+        <v>1271</v>
       </c>
       <c r="B333" t="s">
-        <v>1301</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>1302</v>
+        <v>1273</v>
       </c>
       <c r="B334" t="s">
-        <v>1303</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>1304</v>
+        <v>1275</v>
       </c>
       <c r="B335" t="s">
-        <v>1305</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>1306</v>
+        <v>1277</v>
       </c>
       <c r="B336" t="s">
-        <v>1307</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>1308</v>
+        <v>1279</v>
       </c>
       <c r="B337" t="s">
-        <v>1309</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>1310</v>
+        <v>1281</v>
       </c>
       <c r="B338" t="s">
-        <v>1311</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>1312</v>
+        <v>1283</v>
       </c>
       <c r="B339" t="s">
-        <v>1313</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>1314</v>
+        <v>1285</v>
       </c>
       <c r="B340" t="s">
-        <v>1315</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>1316</v>
+        <v>1287</v>
       </c>
       <c r="B341" t="s">
-        <v>1317</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>1318</v>
+        <v>1289</v>
       </c>
       <c r="B342" t="s">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A343" t="s">
-        <v>1320</v>
-      </c>
-      <c r="B343" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A344" t="s">
-        <v>1322</v>
-      </c>
-      <c r="B344" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A345" t="s">
-        <v>1324</v>
-      </c>
-      <c r="B345" t="s">
-        <v>1325</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A348" s="3" t="s">
-        <v>1356</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A349" s="24" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A345" s="3" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A346" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B349" s="24" t="s">
+      <c r="B346" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B347" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B348" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B349" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>1147</v>
+        <v>1296</v>
       </c>
       <c r="B350" t="s">
-        <v>1357</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>1358</v>
+        <v>1155</v>
       </c>
       <c r="B351" t="s">
-        <v>1359</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>1360</v>
+        <v>1299</v>
       </c>
       <c r="B352" t="s">
-        <v>1361</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>1362</v>
+        <v>1134</v>
       </c>
       <c r="B353" t="s">
-        <v>1363</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>1364</v>
+        <v>1302</v>
       </c>
       <c r="B354" t="s">
-        <v>1371</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>1365</v>
+        <v>1304</v>
       </c>
       <c r="B355" t="s">
-        <v>1366</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>1367</v>
+        <v>1306</v>
       </c>
       <c r="B356" t="s">
-        <v>1368</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>1369</v>
+        <v>1308</v>
       </c>
       <c r="B357" t="s">
-        <v>1372</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>1370</v>
+        <v>1310</v>
       </c>
       <c r="B358" t="s">
-        <v>1373</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A359" s="23"/>
+      <c r="A359" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1313</v>
+      </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" s="23"/>
-    </row>
-    <row r="361" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A361" s="3" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A362" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="B362" s="22" t="s">
-        <v>255</v>
+      <c r="A360" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1319</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>1375</v>
+        <v>1320</v>
       </c>
       <c r="B363" t="s">
-        <v>1159</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>1157</v>
+        <v>1322</v>
       </c>
       <c r="B364" t="s">
-        <v>1376</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>1158</v>
+        <v>1324</v>
       </c>
       <c r="B365" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A366" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B366" t="s">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A367" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B367" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A368" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B368" t="s">
-        <v>1383</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A369" t="s">
-        <v>1384</v>
-      </c>
-      <c r="B369" t="s">
-        <v>1385</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A368" s="3" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A369" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="B369" s="24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>1386</v>
+        <v>1147</v>
       </c>
       <c r="B370" t="s">
-        <v>1387</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>1388</v>
+        <v>1358</v>
       </c>
       <c r="B371" t="s">
-        <v>1389</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>1390</v>
+        <v>1360</v>
       </c>
       <c r="B372" t="s">
-        <v>1391</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>1392</v>
+        <v>1362</v>
       </c>
       <c r="B373" t="s">
-        <v>1437</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>1393</v>
+        <v>1364</v>
       </c>
       <c r="B374" t="s">
-        <v>1438</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>1394</v>
+        <v>1365</v>
       </c>
       <c r="B375" t="s">
-        <v>1439</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>1395</v>
+        <v>1367</v>
       </c>
       <c r="B376" t="s">
-        <v>1440</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>1396</v>
+        <v>1369</v>
       </c>
       <c r="B377" t="s">
-        <v>1441</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>1397</v>
+        <v>1370</v>
       </c>
       <c r="B378" t="s">
-        <v>1442</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A379" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B379" t="s">
-        <v>1443</v>
-      </c>
+      <c r="A379" s="23"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A380" t="s">
-        <v>1399</v>
-      </c>
-      <c r="B380" t="s">
-        <v>1444</v>
+      <c r="A380" s="23"/>
+    </row>
+    <row r="381" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A381" s="3" t="s">
+        <v>1374</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A382" s="25" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A383" s="21" t="s">
+      <c r="A382" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B383" s="22" t="s">
+      <c r="B382" s="22" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1159</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>1145</v>
+        <v>1157</v>
       </c>
       <c r="B384" t="s">
-        <v>1421</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>1417</v>
+        <v>1158</v>
       </c>
       <c r="B385" t="s">
-        <v>1422</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>1423</v>
+        <v>1378</v>
       </c>
       <c r="B386" t="s">
-        <v>1424</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>1425</v>
+        <v>1380</v>
       </c>
       <c r="B387" t="s">
-        <v>1426</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>1427</v>
+        <v>1382</v>
       </c>
       <c r="B388" t="s">
-        <v>1428</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>1429</v>
+        <v>1384</v>
       </c>
       <c r="B389" t="s">
-        <v>1430</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>1431</v>
+        <v>1386</v>
       </c>
       <c r="B390" t="s">
-        <v>1432</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>1419</v>
+        <v>1388</v>
       </c>
       <c r="B391" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="393" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A393" s="25" t="s">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A394" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="B394" s="22" t="s">
-        <v>255</v>
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B392" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1438</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>1445</v>
+        <v>1394</v>
       </c>
       <c r="B395" t="s">
-        <v>1446</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>1405</v>
+        <v>1395</v>
       </c>
       <c r="B396" t="s">
-        <v>1447</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>1407</v>
+        <v>1396</v>
       </c>
       <c r="B397" t="s">
-        <v>1448</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>1403</v>
+        <v>1397</v>
       </c>
       <c r="B398" t="s">
-        <v>1449</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>1409</v>
+        <v>1398</v>
       </c>
       <c r="B399" t="s">
-        <v>1450</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>1451</v>
+        <v>1399</v>
       </c>
       <c r="B400" t="s">
-        <v>1452</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A401" t="s">
-        <v>1453</v>
-      </c>
-      <c r="B401" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A402" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B402" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A405" s="3" t="s">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A406" s="21" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B406" s="22" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A402" s="25" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A403" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="B403" s="22" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B405" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>1145</v>
+        <v>1425</v>
       </c>
       <c r="B407" t="s">
-        <v>1402</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>1403</v>
+        <v>1427</v>
       </c>
       <c r="B408" t="s">
-        <v>1404</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>1405</v>
+        <v>1429</v>
       </c>
       <c r="B409" t="s">
-        <v>1406</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>1407</v>
+        <v>1431</v>
       </c>
       <c r="B410" t="s">
-        <v>1408</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>1409</v>
+        <v>1419</v>
       </c>
       <c r="B411" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A412" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B412" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A413" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B413" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A414" t="s">
-        <v>1413</v>
-      </c>
-      <c r="B414" t="s">
-        <v>1414</v>
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A413" s="25" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A414" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="B414" s="22" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>1415</v>
+        <v>1445</v>
       </c>
       <c r="B415" t="s">
-        <v>1416</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>1417</v>
+        <v>1405</v>
       </c>
       <c r="B416" t="s">
-        <v>1418</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B417" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A425" s="3" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A426" s="21" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B426" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B427" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B428" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B433" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
         <v>1419</v>
       </c>
-      <c r="B417" t="s">
+      <c r="B437" t="s">
         <v>1435</v>
       </c>
     </row>
-    <row r="418" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A418" t="s">
+    <row r="438" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A438" t="s">
         <v>1458</v>
       </c>
-      <c r="B418" t="s">
+      <c r="B438" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A419" t="s">
+    <row r="439" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A439" t="s">
         <v>1457</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new ppt files
</commit_message>
<xml_diff>
--- a/DevOps_Cheatsheet.xlsx
+++ b/DevOps_Cheatsheet.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
     <sheet name="GIT" sheetId="6" r:id="rId2"/>
     <sheet name="Maven" sheetId="2" r:id="rId3"/>
-    <sheet name="Docker" sheetId="5" r:id="rId4"/>
-    <sheet name="K8s" sheetId="3" r:id="rId5"/>
+    <sheet name="Ansible" sheetId="8" r:id="rId4"/>
+    <sheet name="Docker" sheetId="5" r:id="rId5"/>
+    <sheet name="K8s" sheetId="3" r:id="rId6"/>
+    <sheet name="AWS" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="1533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="1534">
   <si>
     <t>CREATING OBJECTS</t>
   </si>
@@ -5855,12 +5857,15 @@
       <t>, ignoring commits that are already in the upstream branch.</t>
     </r>
   </si>
+  <si>
+    <t>ANSIBLE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5978,14 +5983,8 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6041,6 +6040,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF444654"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6168,7 +6173,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -6222,6 +6227,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="8" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -6517,10 +6525,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="79.77734375" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6530,7 +6542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
+    <sheetView topLeftCell="A437" workbookViewId="0">
       <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
@@ -10484,6 +10496,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="88.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B289"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
@@ -12585,7 +12622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B162"/>
   <sheetViews>
@@ -13687,4 +13724,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="2" max="2" width="70.88671875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>